<commit_message>
Agregar exceles para matrices de confusión y curva ROC
</commit_message>
<xml_diff>
--- a/Parte A/Data/resultados_validacion_cruzada.xlsx
+++ b/Parte A/Data/resultados_validacion_cruzada.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6851864761240851</v>
+        <v>0.7011554793401927</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7045577900453635</v>
+        <v>0.6931624611341978</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6828807760570372</v>
+        <v>0.7072593778714615</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7309179854879198</v>
+        <v>0.6815706391498696</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7480236567462425</v>
+        <v>0.7803321918335155</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.711606831648658</v>
+        <v>0.7304915890903152</v>
       </c>
       <c r="C3" t="n">
-        <v>0.719799326626957</v>
+        <v>0.7245803709759692</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7254920394864177</v>
+        <v>0.7372629361108668</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7192213540584474</v>
+        <v>0.7143244425120358</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7857406455849762</v>
+        <v>0.8117229101249219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>